<commit_message>
remove lang local storage & changelog language
</commit_message>
<xml_diff>
--- a/cfg/excel/lang_cfg.xlsx
+++ b/cfg/excel/lang_cfg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Emanon\cfg\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Emanon\cfg\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09CEFA0-D9D6-4D67-AEEC-5910719631F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C499339F-7D24-48B3-B707-610B14E2C37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="3975" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="148">
   <si>
     <t>[TABLE_BEGIN]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -653,6 +651,82 @@
   </si>
   <si>
     <t>進捗バー</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最近更新
+版本号：13.0.0
+发布日期：2025-04-01
+核心更新：
+多语言系统增强
+• 新增日语语言支持（801bda8）
+• 扩展基础语言框架（7ec452e）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recent Update
+Version Number: 13.0.0
+Release Date: April 1, 2025
+Core Updates:
+Enhancement of the Multilingual System
+• Added Japanese language support (801bda8)
+• Extended the basic language framework (7ec452e)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">最近のアップデート
+バージョン番号：13.0.0
+リリース日：2025 年 4 月 1 日
+核心アップデート：
+多言語システムの強化
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・日本語の言語サポートを新たに追加しました</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">（801bda8）
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・基本的な言語フレームワークを拡張しました</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（7ec452e）</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1030,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1567,8 +1641,22 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" ht="108.75" x14ac:dyDescent="0.4">
+      <c r="A39" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>